<commit_message>
Upload Module done for excel
</commit_message>
<xml_diff>
--- a/Test_Run.xlsx
+++ b/Test_Run.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PHP\xampp\htdocs\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PHP\xampp\htdocs\SLMCQ\SLMCQ\ui\test-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Category</t>
   </si>
@@ -50,18 +50,6 @@
     <t>Which keyword is used for exception handling?</t>
   </si>
   <si>
-    <t>super</t>
-  </si>
-  <si>
-    <t>this</t>
-  </si>
-  <si>
-    <t>finalize</t>
-  </si>
-  <si>
-    <t>try</t>
-  </si>
-  <si>
     <t>Match the correct pair</t>
   </si>
   <si>
@@ -80,9 +68,6 @@
     <t>Option 8</t>
   </si>
   <si>
-    <t>char</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -110,9 +95,6 @@
     <t>Fill In the blanks with proper article</t>
   </si>
   <si>
-    <t>%blank% dog came running towards cynthia . Looking at %blank% Cynthia got scared.</t>
-  </si>
-  <si>
     <t>a,the</t>
   </si>
   <si>
@@ -129,6 +111,18 @@
   </si>
   <si>
     <t>FIB</t>
+  </si>
+  <si>
+    <t>1.png</t>
+  </si>
+  <si>
+    <t>2.png</t>
+  </si>
+  <si>
+    <t>3.png</t>
+  </si>
+  <si>
+    <t>4.png</t>
   </si>
 </sst>
 </file>
@@ -452,7 +446,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,13 +460,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -487,19 +481,19 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -510,7 +504,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -519,16 +513,16 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -536,37 +530,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -574,16 +568,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>